<commit_message>
made a minor change on project description.
</commit_message>
<xml_diff>
--- a/data/Raw data dictionary.xlsx
+++ b/data/Raw data dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51fa0a69fdf335f8/Research/PaST pilot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FilesVC\PaST-pilot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC104899311E477C5ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E7AFE47-F4C5-4EFC-AEBB-1F8B0CC5ACEE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5762B8F-B528-4A17-94E3-461D76A92543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>